<commit_message>
Start cleaning up GHGSat data, errors with importing. Pausing to update PyCharm
</commit_message>
<xml_diff>
--- a/00_raw_data/SciAv_Stage1_submitted-2023-02-21.xlsx
+++ b/00_raw_data/SciAv_Stage1_submitted-2023-02-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://championx.sharepoint.com/sites/EM-US-SCA-FlightData/Flights/Stanford/Final Submitted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{C1AF4DA0-19D2-4184-9665-412D6C5CF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD9AA7C-AF15-42FD-810C-FFC73D2C9972}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43664A62-C3DE-6D4D-A3F9-92953E0900BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
+    <workbookView xWindow="37300" yWindow="2220" windowWidth="29040" windowHeight="15840" xr2:uid="{AC3A3917-1DB8-476E-8C07-EEBD570C7043}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Table" sheetId="12" r:id="rId1"/>
@@ -262,6 +262,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -270,15 +279,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,65 +597,65 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="4" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="11" customWidth="1"/>
     <col min="6" max="6" width="13" style="6" customWidth="1"/>
     <col min="7" max="7" width="13" style="8" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="15.83203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="10" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
         <v>6</v>
       </c>
@@ -674,7 +674,7 @@
       <c r="F3" s="9">
         <v>205</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="14">
         <v>8.1999999999999993</v>
       </c>
       <c r="H3" s="9">
@@ -687,7 +687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>7</v>
       </c>
@@ -706,7 +706,7 @@
       <c r="F4" s="9">
         <v>207</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="14">
         <v>7.2</v>
       </c>
       <c r="H4" s="9">
@@ -719,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>8</v>
       </c>
@@ -738,7 +738,7 @@
       <c r="F5" s="9">
         <v>209</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="14">
         <v>7.6</v>
       </c>
       <c r="H5" s="9">
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>9</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="F6" s="9">
         <v>206</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="14">
         <v>7.8</v>
       </c>
       <c r="H6" s="9">
@@ -783,10 +783,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>1</v>
       </c>
@@ -815,7 +815,7 @@
         <v>66488</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>2</v>
       </c>
@@ -846,7 +846,7 @@
         <v>69277</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -875,7 +875,7 @@
         <v>71461</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -904,7 +904,7 @@
         <v>73443</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>5</v>
       </c>
@@ -935,7 +935,7 @@
         <v>76377</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>6</v>
       </c>
@@ -964,7 +964,7 @@
         <v>78637</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>7</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="F14" s="9">
         <v>318</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="14">
         <v>4</v>
       </c>
       <c r="H14" s="9">
@@ -996,10 +996,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>70064</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>72350</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>3</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="F18" s="9">
         <v>24</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="14">
         <v>4.4000000000000004</v>
       </c>
       <c r="H18" s="9">
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>76586</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>78502</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>6</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>83042</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="F22" s="9">
         <v>325</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="14">
         <v>5.3</v>
       </c>
       <c r="H22" s="9">
@@ -1231,6 +1231,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF4A7E0C1C09E0408DE2334E76E485FD" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0b9d783383bc6aafecc7f20faaede2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d753306e-285a-44c6-8280-85ac401334a2" xmlns:ns3="fc353d8b-3dd1-4c08-8d95-c533a13405a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31f00eeba95c506051609f8103a99647" ns2:_="" ns3:_="">
     <xsd:import namespace="d753306e-285a-44c6-8280-85ac401334a2"/>
@@ -1473,17 +1484,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d753306e-285a-44c6-8280-85ac401334a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fc353d8b-3dd1-4c08-8d95-c533a13405a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1494,6 +1494,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D40DFC-9657-4687-8074-E99047F72E77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1512,23 +1529,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E41E6AA-2334-497B-8624-E455A3B4F725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d753306e-285a-44c6-8280-85ac401334a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc353d8b-3dd1-4c08-8d95-c533a13405a8"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8368B9D-8C4E-4762-9B15-D62B6087258A}">
   <ds:schemaRefs>

</xml_diff>